<commit_message>
Auto update ESO load data
</commit_message>
<xml_diff>
--- a/data/plexos_load_master.xlsx
+++ b/data/plexos_load_master.xlsx
@@ -566,79 +566,79 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D2" t="n">
-        <v>4935</v>
+        <v>4874</v>
       </c>
       <c r="E2" t="n">
-        <v>4618</v>
+        <v>4559</v>
       </c>
       <c r="F2" t="n">
-        <v>4581</v>
+        <v>4523</v>
       </c>
       <c r="G2" t="n">
-        <v>4611</v>
+        <v>4553</v>
       </c>
       <c r="H2" t="n">
-        <v>4624</v>
+        <v>4566</v>
       </c>
       <c r="I2" t="n">
-        <v>4757</v>
+        <v>4698</v>
       </c>
       <c r="J2" t="n">
-        <v>5280</v>
+        <v>5216</v>
       </c>
       <c r="K2" t="n">
-        <v>5896</v>
+        <v>5828</v>
       </c>
       <c r="L2" t="n">
-        <v>6431</v>
+        <v>6358</v>
       </c>
       <c r="M2" t="n">
-        <v>6578</v>
+        <v>6504</v>
       </c>
       <c r="N2" t="n">
-        <v>6506</v>
+        <v>6429</v>
       </c>
       <c r="O2" t="n">
-        <v>6434</v>
+        <v>6353</v>
       </c>
       <c r="P2" t="n">
-        <v>6324</v>
+        <v>6238</v>
       </c>
       <c r="Q2" t="n">
-        <v>6257</v>
+        <v>6167</v>
       </c>
       <c r="R2" t="n">
-        <v>6180</v>
+        <v>6085</v>
       </c>
       <c r="S2" t="n">
-        <v>6155</v>
+        <v>6059</v>
       </c>
       <c r="T2" t="n">
-        <v>6199</v>
+        <v>6105</v>
       </c>
       <c r="U2" t="n">
-        <v>6346</v>
+        <v>6258</v>
       </c>
       <c r="V2" t="n">
-        <v>6516</v>
+        <v>6435</v>
       </c>
       <c r="W2" t="n">
-        <v>6503</v>
+        <v>6422</v>
       </c>
       <c r="X2" t="n">
-        <v>6277</v>
+        <v>6198</v>
       </c>
       <c r="Y2" t="n">
-        <v>5991</v>
+        <v>5914</v>
       </c>
       <c r="Z2" t="n">
-        <v>5736</v>
+        <v>5662</v>
       </c>
       <c r="AA2" t="n">
-        <v>5344</v>
+        <v>5274</v>
       </c>
     </row>
     <row r="3">
@@ -649,79 +649,79 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D3" t="n">
-        <v>4874</v>
+        <v>4832</v>
       </c>
       <c r="E3" t="n">
-        <v>4559</v>
+        <v>4519</v>
       </c>
       <c r="F3" t="n">
-        <v>4523</v>
+        <v>4483</v>
       </c>
       <c r="G3" t="n">
-        <v>4553</v>
+        <v>4513</v>
       </c>
       <c r="H3" t="n">
-        <v>4566</v>
+        <v>4526</v>
       </c>
       <c r="I3" t="n">
-        <v>4698</v>
+        <v>4657</v>
       </c>
       <c r="J3" t="n">
-        <v>5216</v>
+        <v>5173</v>
       </c>
       <c r="K3" t="n">
-        <v>5828</v>
+        <v>5781</v>
       </c>
       <c r="L3" t="n">
-        <v>6358</v>
+        <v>6309</v>
       </c>
       <c r="M3" t="n">
-        <v>6504</v>
+        <v>6454</v>
       </c>
       <c r="N3" t="n">
-        <v>6429</v>
+        <v>6376</v>
       </c>
       <c r="O3" t="n">
-        <v>6353</v>
+        <v>6297</v>
       </c>
       <c r="P3" t="n">
-        <v>6238</v>
+        <v>6178</v>
       </c>
       <c r="Q3" t="n">
-        <v>6167</v>
+        <v>6105</v>
       </c>
       <c r="R3" t="n">
-        <v>6085</v>
+        <v>6021</v>
       </c>
       <c r="S3" t="n">
-        <v>6059</v>
+        <v>5994</v>
       </c>
       <c r="T3" t="n">
-        <v>6105</v>
+        <v>6031</v>
       </c>
       <c r="U3" t="n">
-        <v>6258</v>
+        <v>6155</v>
       </c>
       <c r="V3" t="n">
-        <v>6435</v>
+        <v>6299</v>
       </c>
       <c r="W3" t="n">
-        <v>6422</v>
+        <v>6287</v>
       </c>
       <c r="X3" t="n">
-        <v>6198</v>
+        <v>6070</v>
       </c>
       <c r="Y3" t="n">
-        <v>5914</v>
+        <v>5796</v>
       </c>
       <c r="Z3" t="n">
-        <v>5662</v>
+        <v>5552</v>
       </c>
       <c r="AA3" t="n">
-        <v>5274</v>
+        <v>5178</v>
       </c>
     </row>
     <row r="4">
@@ -732,79 +732,79 @@
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D4" t="n">
-        <v>4832</v>
+        <v>4946</v>
       </c>
       <c r="E4" t="n">
-        <v>4519</v>
+        <v>4685</v>
       </c>
       <c r="F4" t="n">
-        <v>4483</v>
+        <v>4561</v>
       </c>
       <c r="G4" t="n">
-        <v>4513</v>
+        <v>4536</v>
       </c>
       <c r="H4" t="n">
-        <v>4526</v>
+        <v>4564</v>
       </c>
       <c r="I4" t="n">
-        <v>4657</v>
+        <v>4637</v>
       </c>
       <c r="J4" t="n">
-        <v>5173</v>
+        <v>4796</v>
       </c>
       <c r="K4" t="n">
-        <v>5781</v>
+        <v>5098</v>
       </c>
       <c r="L4" t="n">
-        <v>6309</v>
+        <v>5766</v>
       </c>
       <c r="M4" t="n">
-        <v>6454</v>
+        <v>6219</v>
       </c>
       <c r="N4" t="n">
-        <v>6376</v>
+        <v>6307</v>
       </c>
       <c r="O4" t="n">
-        <v>6297</v>
+        <v>6231</v>
       </c>
       <c r="P4" t="n">
-        <v>6178</v>
+        <v>6145</v>
       </c>
       <c r="Q4" t="n">
-        <v>6105</v>
+        <v>6041</v>
       </c>
       <c r="R4" t="n">
-        <v>6021</v>
+        <v>5955</v>
       </c>
       <c r="S4" t="n">
-        <v>5994</v>
+        <v>5961</v>
       </c>
       <c r="T4" t="n">
-        <v>6031</v>
+        <v>6036</v>
       </c>
       <c r="U4" t="n">
-        <v>6155</v>
+        <v>6184</v>
       </c>
       <c r="V4" t="n">
-        <v>6299</v>
+        <v>6264</v>
       </c>
       <c r="W4" t="n">
-        <v>6287</v>
+        <v>6133</v>
       </c>
       <c r="X4" t="n">
-        <v>6070</v>
+        <v>5895</v>
       </c>
       <c r="Y4" t="n">
-        <v>5796</v>
+        <v>5619</v>
       </c>
       <c r="Z4" t="n">
-        <v>5552</v>
+        <v>5493</v>
       </c>
       <c r="AA4" t="n">
-        <v>5178</v>
+        <v>5223</v>
       </c>
     </row>
     <row r="5">
@@ -812,82 +812,82 @@
         <v>2026</v>
       </c>
       <c r="B5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" t="n">
         <v>1</v>
       </c>
-      <c r="C5" t="n">
-        <v>31</v>
-      </c>
       <c r="D5" t="n">
-        <v>4946</v>
+        <v>5071</v>
       </c>
       <c r="E5" t="n">
-        <v>4685</v>
+        <v>4847</v>
       </c>
       <c r="F5" t="n">
-        <v>4561</v>
+        <v>4753</v>
       </c>
       <c r="G5" t="n">
-        <v>4536</v>
+        <v>4699</v>
       </c>
       <c r="H5" t="n">
-        <v>4564</v>
+        <v>4671</v>
       </c>
       <c r="I5" t="n">
-        <v>4637</v>
+        <v>4758</v>
       </c>
       <c r="J5" t="n">
-        <v>4796</v>
+        <v>4918</v>
       </c>
       <c r="K5" t="n">
-        <v>5098</v>
+        <v>5269</v>
       </c>
       <c r="L5" t="n">
         <v>5766</v>
       </c>
       <c r="M5" t="n">
-        <v>6219</v>
+        <v>6257</v>
       </c>
       <c r="N5" t="n">
-        <v>6307</v>
+        <v>6466</v>
       </c>
       <c r="O5" t="n">
-        <v>6231</v>
+        <v>6423</v>
       </c>
       <c r="P5" t="n">
-        <v>6145</v>
+        <v>6344</v>
       </c>
       <c r="Q5" t="n">
-        <v>6041</v>
+        <v>6230</v>
       </c>
       <c r="R5" t="n">
-        <v>5955</v>
+        <v>6144</v>
       </c>
       <c r="S5" t="n">
-        <v>5961</v>
+        <v>6169</v>
       </c>
       <c r="T5" t="n">
-        <v>6036</v>
+        <v>6295</v>
       </c>
       <c r="U5" t="n">
-        <v>6184</v>
+        <v>6522</v>
       </c>
       <c r="V5" t="n">
-        <v>6264</v>
+        <v>6660</v>
       </c>
       <c r="W5" t="n">
-        <v>6133</v>
+        <v>6587</v>
       </c>
       <c r="X5" t="n">
-        <v>5895</v>
+        <v>6373</v>
       </c>
       <c r="Y5" t="n">
-        <v>5619</v>
+        <v>6078</v>
       </c>
       <c r="Z5" t="n">
-        <v>5493</v>
+        <v>5871</v>
       </c>
       <c r="AA5" t="n">
-        <v>5223</v>
+        <v>5505</v>
       </c>
     </row>
     <row r="6">
@@ -898,79 +898,79 @@
         <v>2</v>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" t="n">
-        <v>5071</v>
+        <v>5277</v>
       </c>
       <c r="E6" t="n">
-        <v>4847</v>
+        <v>5024</v>
       </c>
       <c r="F6" t="n">
-        <v>4753</v>
+        <v>4907</v>
       </c>
       <c r="G6" t="n">
-        <v>4699</v>
+        <v>4929</v>
       </c>
       <c r="H6" t="n">
-        <v>4671</v>
+        <v>5025</v>
       </c>
       <c r="I6" t="n">
-        <v>4758</v>
+        <v>5199</v>
       </c>
       <c r="J6" t="n">
-        <v>4918</v>
+        <v>5732</v>
       </c>
       <c r="K6" t="n">
-        <v>5269</v>
+        <v>6368</v>
       </c>
       <c r="L6" t="n">
-        <v>5766</v>
+        <v>6931</v>
       </c>
       <c r="M6" t="n">
-        <v>6257</v>
+        <v>7118</v>
       </c>
       <c r="N6" t="n">
-        <v>6466</v>
+        <v>6994</v>
       </c>
       <c r="O6" t="n">
-        <v>6423</v>
+        <v>6860</v>
       </c>
       <c r="P6" t="n">
-        <v>6344</v>
+        <v>6708</v>
       </c>
       <c r="Q6" t="n">
-        <v>6230</v>
+        <v>6652</v>
       </c>
       <c r="R6" t="n">
-        <v>6144</v>
+        <v>6602</v>
       </c>
       <c r="S6" t="n">
-        <v>6169</v>
+        <v>6619</v>
       </c>
       <c r="T6" t="n">
-        <v>6295</v>
+        <v>6636</v>
       </c>
       <c r="U6" t="n">
-        <v>6522</v>
+        <v>6811</v>
       </c>
       <c r="V6" t="n">
-        <v>6660</v>
+        <v>7037</v>
       </c>
       <c r="W6" t="n">
-        <v>6587</v>
+        <v>7007</v>
       </c>
       <c r="X6" t="n">
-        <v>6373</v>
+        <v>6802</v>
       </c>
       <c r="Y6" t="n">
-        <v>6078</v>
+        <v>6514</v>
       </c>
       <c r="Z6" t="n">
-        <v>5871</v>
+        <v>6252</v>
       </c>
       <c r="AA6" t="n">
-        <v>5505</v>
+        <v>5837</v>
       </c>
     </row>
     <row r="7">
@@ -981,79 +981,79 @@
         <v>2</v>
       </c>
       <c r="C7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7" t="n">
-        <v>5277</v>
+        <v>5385</v>
       </c>
       <c r="E7" t="n">
-        <v>5024</v>
+        <v>5072</v>
       </c>
       <c r="F7" t="n">
-        <v>4907</v>
+        <v>5036</v>
       </c>
       <c r="G7" t="n">
-        <v>4929</v>
+        <v>5068</v>
       </c>
       <c r="H7" t="n">
-        <v>5025</v>
+        <v>5082</v>
       </c>
       <c r="I7" t="n">
-        <v>5199</v>
+        <v>5224</v>
       </c>
       <c r="J7" t="n">
-        <v>5732</v>
+        <v>5783</v>
       </c>
       <c r="K7" t="n">
-        <v>6368</v>
+        <v>6442</v>
       </c>
       <c r="L7" t="n">
-        <v>6931</v>
+        <v>7013</v>
       </c>
       <c r="M7" t="n">
-        <v>7118</v>
+        <v>7171</v>
       </c>
       <c r="N7" t="n">
-        <v>6994</v>
+        <v>7081</v>
       </c>
       <c r="O7" t="n">
-        <v>6860</v>
+        <v>6989</v>
       </c>
       <c r="P7" t="n">
-        <v>6708</v>
+        <v>6851</v>
       </c>
       <c r="Q7" t="n">
-        <v>6652</v>
+        <v>6766</v>
       </c>
       <c r="R7" t="n">
-        <v>6602</v>
+        <v>6669</v>
       </c>
       <c r="S7" t="n">
-        <v>6619</v>
+        <v>6638</v>
       </c>
       <c r="T7" t="n">
-        <v>6636</v>
+        <v>6693</v>
       </c>
       <c r="U7" t="n">
-        <v>6811</v>
+        <v>6876</v>
       </c>
       <c r="V7" t="n">
-        <v>7037</v>
+        <v>7088</v>
       </c>
       <c r="W7" t="n">
-        <v>7007</v>
+        <v>7075</v>
       </c>
       <c r="X7" t="n">
-        <v>6802</v>
+        <v>6844</v>
       </c>
       <c r="Y7" t="n">
-        <v>6514</v>
+        <v>6552</v>
       </c>
       <c r="Z7" t="n">
-        <v>6252</v>
+        <v>6291</v>
       </c>
       <c r="AA7" t="n">
-        <v>5837</v>
+        <v>5891</v>
       </c>
     </row>
   </sheetData>

</xml_diff>